<commit_message>
adding log4j and stepDef
</commit_message>
<xml_diff>
--- a/testSuite.xlsx
+++ b/testSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idnkiw\Desktop\Vaibhav\MVNExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1926CBD-5E5A-481D-960F-09788B56A353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50B3097-DA25-4764-A749-BB33BF156D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Test_ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Validate login with valid username and password</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>LaunchApplication</t>
   </si>
   <si>
@@ -74,6 +71,12 @@
   </si>
   <si>
     <t>KeyWords</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -391,9 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -433,30 +438,30 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -464,33 +469,67 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +542,7 @@
           <x14:formula1>
             <xm:f>keyWords!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D5 D8:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -526,17 +565,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding reflection api to invoke steps from specific classes
</commit_message>
<xml_diff>
--- a/testSuite.xlsx
+++ b/testSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idnkiw\Desktop\Vaibhav\MVNExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50B3097-DA25-4764-A749-BB33BF156D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81C3BCA-0AA3-4D13-A252-698A6F2FDEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sanity" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Test_ID</t>
   </si>
@@ -76,7 +76,13 @@
     <t>admin2</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>com.sbn.pages.StepDefs</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -552,30 +558,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7413A2DC-4B70-4A3E-B169-50B2DC460223}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>